<commit_message>
finished. Possible loading animations and error handling.
</commit_message>
<xml_diff>
--- a/Sifh.ReportGenerator/Excel Templates/Templates.xlsx
+++ b/Sifh.ReportGenerator/Excel Templates/Templates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilherme\source\repos\brendongreene\Sifh.ReportGenerator\Sifh.ReportGenerator\Excel Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A8CA89-EA51-486C-A3BA-A812B9B7928C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F606DC03-3BCD-4085-9CFE-97D1E3EE598A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{997B08C3-0059-4A02-89AB-DD06527C47E4}"/>
+    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{997B08C3-0059-4A02-89AB-DD06527C47E4}"/>
   </bookViews>
   <sheets>
     <sheet name="MCC" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
   <si>
     <t>Wild Capture Fishery (Complete Section 2)</t>
   </si>
@@ -370,15 +370,22 @@
   <si>
     <t>*Note: A Lot Identifier is generated by the shipper based on its cargo tracking and record-keeping protocols.</t>
   </si>
+  <si>
+    <t>THUNNUS ALBACARE</t>
+  </si>
+  <si>
+    <t>YFT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#."/>
+    <numFmt numFmtId="165" formatCode="000\ 0000\ 0000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,6 +535,14 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -715,7 +730,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1108,117 +1123,132 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1231,15 +1261,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1303,10 +1324,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3107,8 +3149,8 @@
   </sheetPr>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A3" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3588,7 +3630,9 @@
       <c r="B29" s="13">
         <v>1</v>
       </c>
-      <c r="C29" s="82"/>
+      <c r="C29" s="82" t="s">
+        <v>88</v>
+      </c>
       <c r="D29" s="82"/>
       <c r="E29" s="82"/>
       <c r="F29" s="83"/>
@@ -3830,8 +3874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20F6DE1E-C4D7-4581-B13B-2767FFCE0CBB}">
   <dimension ref="C1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:H11"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30:M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3848,7 +3892,7 @@
     <col min="12" max="12" width="13.7109375" customWidth="1"/>
     <col min="13" max="13" width="9.5703125" customWidth="1"/>
     <col min="14" max="14" width="45.5703125" customWidth="1"/>
-    <col min="15" max="15" width="29.28515625" customWidth="1"/>
+    <col min="15" max="15" width="35.42578125" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
   </cols>
@@ -3856,67 +3900,67 @@
     <row r="1" spans="3:15" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C3" s="164" t="s">
+      <c r="C3" s="165" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="165"/>
-      <c r="E3" s="165"/>
-      <c r="F3" s="165"/>
-      <c r="G3" s="165"/>
-      <c r="H3" s="165"/>
-      <c r="I3" s="165"/>
-      <c r="J3" s="165"/>
-      <c r="K3" s="165"/>
-      <c r="L3" s="165"/>
-      <c r="M3" s="165"/>
-      <c r="N3" s="165"/>
-      <c r="O3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
+      <c r="L3" s="166"/>
+      <c r="M3" s="166"/>
+      <c r="N3" s="166"/>
+      <c r="O3" s="167"/>
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C4" s="167"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="168"/>
-      <c r="G4" s="168"/>
-      <c r="H4" s="168"/>
-      <c r="I4" s="168"/>
-      <c r="J4" s="168"/>
-      <c r="K4" s="168"/>
-      <c r="L4" s="168"/>
-      <c r="M4" s="168"/>
-      <c r="N4" s="168"/>
-      <c r="O4" s="169"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="169"/>
+      <c r="F4" s="169"/>
+      <c r="G4" s="169"/>
+      <c r="H4" s="169"/>
+      <c r="I4" s="169"/>
+      <c r="J4" s="169"/>
+      <c r="K4" s="169"/>
+      <c r="L4" s="169"/>
+      <c r="M4" s="169"/>
+      <c r="N4" s="169"/>
+      <c r="O4" s="170"/>
     </row>
     <row r="5" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="170"/>
-      <c r="D5" s="171"/>
-      <c r="E5" s="171"/>
-      <c r="F5" s="171"/>
-      <c r="G5" s="171"/>
-      <c r="H5" s="171"/>
-      <c r="I5" s="171"/>
-      <c r="J5" s="171"/>
-      <c r="K5" s="171"/>
-      <c r="L5" s="171"/>
-      <c r="M5" s="171"/>
-      <c r="N5" s="171"/>
-      <c r="O5" s="172"/>
+      <c r="C5" s="171"/>
+      <c r="D5" s="172"/>
+      <c r="E5" s="172"/>
+      <c r="F5" s="172"/>
+      <c r="G5" s="172"/>
+      <c r="H5" s="172"/>
+      <c r="I5" s="172"/>
+      <c r="J5" s="172"/>
+      <c r="K5" s="172"/>
+      <c r="L5" s="172"/>
+      <c r="M5" s="172"/>
+      <c r="N5" s="172"/>
+      <c r="O5" s="173"/>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="33"/>
-      <c r="D6" s="163" t="s">
+      <c r="D6" s="164" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="163"/>
-      <c r="H6" s="163"/>
-      <c r="I6" s="163"/>
-      <c r="J6" s="163"/>
-      <c r="K6" s="163"/>
-      <c r="L6" s="163"/>
-      <c r="M6" s="163"/>
-      <c r="N6" s="163"/>
+      <c r="E6" s="164"/>
+      <c r="F6" s="164"/>
+      <c r="G6" s="164"/>
+      <c r="H6" s="164"/>
+      <c r="I6" s="164"/>
+      <c r="J6" s="164"/>
+      <c r="K6" s="164"/>
+      <c r="L6" s="164"/>
+      <c r="M6" s="164"/>
+      <c r="N6" s="164"/>
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="3:15" x14ac:dyDescent="0.25">
@@ -3939,53 +3983,53 @@
     </row>
     <row r="9" spans="3:15" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C9" s="35"/>
-      <c r="D9" s="163" t="s">
+      <c r="D9" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="163"/>
-      <c r="H9" s="173"/>
-      <c r="I9" s="186" t="s">
+      <c r="E9" s="164"/>
+      <c r="F9" s="164"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="174"/>
+      <c r="I9" s="191" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="163"/>
-      <c r="K9" s="163"/>
-      <c r="L9" s="163"/>
-      <c r="M9" s="163"/>
-      <c r="N9" s="163"/>
-      <c r="O9" s="173"/>
+      <c r="J9" s="164"/>
+      <c r="K9" s="164"/>
+      <c r="L9" s="164"/>
+      <c r="M9" s="164"/>
+      <c r="N9" s="164"/>
+      <c r="O9" s="174"/>
     </row>
     <row r="10" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C10" s="4"/>
-      <c r="D10" s="185" t="s">
+      <c r="D10" s="190" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="213"/>
-      <c r="F10" s="213"/>
-      <c r="G10" s="213"/>
-      <c r="H10" s="214"/>
-      <c r="I10" s="150"/>
-      <c r="J10" s="148"/>
-      <c r="K10" s="148"/>
-      <c r="L10" s="148"/>
-      <c r="M10" s="148"/>
-      <c r="N10" s="148"/>
+      <c r="E10" s="188"/>
+      <c r="F10" s="188"/>
+      <c r="G10" s="188"/>
+      <c r="H10" s="189"/>
+      <c r="I10" s="185"/>
+      <c r="J10" s="178"/>
+      <c r="K10" s="178"/>
+      <c r="L10" s="178"/>
+      <c r="M10" s="178"/>
+      <c r="N10" s="178"/>
       <c r="O10" s="5"/>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C11" s="27"/>
-      <c r="D11" s="185"/>
-      <c r="E11" s="213"/>
-      <c r="F11" s="213"/>
-      <c r="G11" s="213"/>
-      <c r="H11" s="214"/>
-      <c r="I11" s="150"/>
-      <c r="J11" s="148"/>
-      <c r="K11" s="148"/>
-      <c r="L11" s="148"/>
-      <c r="M11" s="148"/>
-      <c r="N11" s="148"/>
+      <c r="D11" s="190"/>
+      <c r="E11" s="188"/>
+      <c r="F11" s="188"/>
+      <c r="G11" s="188"/>
+      <c r="H11" s="189"/>
+      <c r="I11" s="185"/>
+      <c r="J11" s="178"/>
+      <c r="K11" s="178"/>
+      <c r="L11" s="178"/>
+      <c r="M11" s="178"/>
+      <c r="N11" s="178"/>
       <c r="O11" s="5"/>
     </row>
     <row r="12" spans="3:15" ht="33.75" x14ac:dyDescent="0.25">
@@ -4017,19 +4061,19 @@
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C14" s="45"/>
-      <c r="D14" s="174" t="s">
+      <c r="D14" s="175" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="175"/>
-      <c r="F14" s="175"/>
-      <c r="G14" s="175"/>
-      <c r="H14" s="176"/>
+      <c r="E14" s="176"/>
+      <c r="F14" s="176"/>
+      <c r="G14" s="176"/>
+      <c r="H14" s="177"/>
       <c r="I14" s="161" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="174"/>
-      <c r="K14" s="174"/>
-      <c r="L14" s="174"/>
+      <c r="J14" s="175"/>
+      <c r="K14" s="175"/>
+      <c r="L14" s="175"/>
       <c r="M14" s="162"/>
       <c r="N14" s="33" t="s">
         <v>58</v>
@@ -4040,54 +4084,54 @@
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C15" s="4"/>
-      <c r="D15" s="148" t="s">
+      <c r="D15" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="177"/>
-      <c r="F15" s="177"/>
-      <c r="G15" s="177"/>
-      <c r="H15" s="178"/>
-      <c r="I15" s="179" t="s">
+      <c r="E15" s="179"/>
+      <c r="F15" s="179"/>
+      <c r="G15" s="179"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="181" t="s">
         <v>49</v>
       </c>
-      <c r="J15" s="180"/>
-      <c r="K15" s="180"/>
-      <c r="L15" s="180"/>
-      <c r="M15" s="181"/>
-      <c r="N15" s="184">
+      <c r="J15" s="182"/>
+      <c r="K15" s="182"/>
+      <c r="L15" s="182"/>
+      <c r="M15" s="183"/>
+      <c r="N15" s="187">
         <v>10398004506</v>
       </c>
       <c r="O15" s="57"/>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
-      <c r="D16" s="177"/>
-      <c r="E16" s="177"/>
-      <c r="F16" s="177"/>
-      <c r="G16" s="177"/>
-      <c r="H16" s="178"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="180"/>
-      <c r="K16" s="180"/>
-      <c r="L16" s="180"/>
-      <c r="M16" s="181"/>
-      <c r="N16" s="184"/>
+      <c r="D16" s="179"/>
+      <c r="E16" s="179"/>
+      <c r="F16" s="179"/>
+      <c r="G16" s="179"/>
+      <c r="H16" s="180"/>
+      <c r="I16" s="184"/>
+      <c r="J16" s="182"/>
+      <c r="K16" s="182"/>
+      <c r="L16" s="182"/>
+      <c r="M16" s="183"/>
+      <c r="N16" s="187"/>
       <c r="O16" s="49"/>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="46"/>
-      <c r="D17" s="177"/>
-      <c r="E17" s="177"/>
-      <c r="F17" s="177"/>
-      <c r="G17" s="177"/>
-      <c r="H17" s="178"/>
-      <c r="I17" s="150" t="s">
+      <c r="D17" s="179"/>
+      <c r="E17" s="179"/>
+      <c r="F17" s="179"/>
+      <c r="G17" s="179"/>
+      <c r="H17" s="180"/>
+      <c r="I17" s="185" t="s">
         <v>50</v>
       </c>
       <c r="J17" s="120"/>
       <c r="K17" s="120"/>
       <c r="L17" s="120"/>
-      <c r="M17" s="183"/>
+      <c r="M17" s="186"/>
       <c r="N17" s="46"/>
       <c r="O17" s="53" t="s">
         <v>47</v>
@@ -4159,7 +4203,9 @@
       <c r="L21" s="148"/>
       <c r="M21" s="148"/>
       <c r="N21" s="149"/>
-      <c r="O21" s="49"/>
+      <c r="O21" s="163">
+        <v>1750102610</v>
+      </c>
     </row>
     <row r="22" spans="3:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="C22" s="24"/>
@@ -4174,7 +4220,7 @@
       <c r="L22" s="148"/>
       <c r="M22" s="148"/>
       <c r="N22" s="149"/>
-      <c r="O22" s="49"/>
+      <c r="O22" s="163"/>
     </row>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="4"/>
@@ -4259,24 +4305,24 @@
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C28" s="38"/>
-      <c r="D28" s="163" t="s">
+      <c r="D28" s="164" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="186" t="s">
+      <c r="E28" s="164"/>
+      <c r="F28" s="164"/>
+      <c r="G28" s="164"/>
+      <c r="H28" s="164"/>
+      <c r="I28" s="191" t="s">
         <v>61</v>
       </c>
-      <c r="J28" s="163"/>
-      <c r="K28" s="163"/>
-      <c r="L28" s="163"/>
-      <c r="M28" s="173"/>
-      <c r="N28" s="163" t="s">
+      <c r="J28" s="164"/>
+      <c r="K28" s="164"/>
+      <c r="L28" s="164"/>
+      <c r="M28" s="174"/>
+      <c r="N28" s="164" t="s">
         <v>56</v>
       </c>
-      <c r="O28" s="173"/>
+      <c r="O28" s="174"/>
     </row>
     <row r="29" spans="3:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C29" s="13"/>
@@ -4287,11 +4333,11 @@
       </c>
       <c r="G29" s="61"/>
       <c r="H29" s="62"/>
-      <c r="I29" s="179"/>
-      <c r="J29" s="187"/>
-      <c r="K29" s="187"/>
-      <c r="L29" s="187"/>
-      <c r="M29" s="188"/>
+      <c r="I29" s="181"/>
+      <c r="J29" s="192"/>
+      <c r="K29" s="192"/>
+      <c r="L29" s="192"/>
+      <c r="M29" s="193"/>
       <c r="N29" s="63" t="s">
         <v>27</v>
       </c>
@@ -4304,11 +4350,11 @@
       <c r="F30" s="60"/>
       <c r="G30" s="41"/>
       <c r="H30" s="42"/>
-      <c r="I30" s="189"/>
-      <c r="J30" s="190"/>
-      <c r="K30" s="190"/>
-      <c r="L30" s="190"/>
-      <c r="M30" s="191"/>
+      <c r="I30" s="215"/>
+      <c r="J30" s="216"/>
+      <c r="K30" s="216"/>
+      <c r="L30" s="216"/>
+      <c r="M30" s="217"/>
       <c r="N30" s="41"/>
       <c r="O30" s="8"/>
     </row>
@@ -4327,7 +4373,7 @@
       <c r="L31" s="120"/>
       <c r="M31" s="120"/>
       <c r="N31" s="120"/>
-      <c r="O31" s="183"/>
+      <c r="O31" s="186"/>
     </row>
     <row r="32" spans="3:15" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
       <c r="C32" s="13"/>
@@ -4348,21 +4394,21 @@
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C33" s="38"/>
-      <c r="D33" s="163" t="s">
+      <c r="D33" s="164" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="163"/>
-      <c r="F33" s="163"/>
-      <c r="G33" s="163"/>
-      <c r="H33" s="163"/>
-      <c r="I33" s="163"/>
-      <c r="J33" s="163"/>
-      <c r="K33" s="173"/>
-      <c r="L33" s="186" t="s">
+      <c r="E33" s="164"/>
+      <c r="F33" s="164"/>
+      <c r="G33" s="164"/>
+      <c r="H33" s="164"/>
+      <c r="I33" s="164"/>
+      <c r="J33" s="164"/>
+      <c r="K33" s="174"/>
+      <c r="L33" s="191" t="s">
         <v>64</v>
       </c>
-      <c r="M33" s="163"/>
-      <c r="N33" s="173"/>
+      <c r="M33" s="164"/>
+      <c r="N33" s="174"/>
       <c r="O33" s="58" t="s">
         <v>55</v>
       </c>
@@ -4419,7 +4465,7 @@
       <c r="O36" s="75"/>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="40">
     <mergeCell ref="N28:O28"/>
     <mergeCell ref="D33:K33"/>
     <mergeCell ref="L33:N33"/>
@@ -4453,6 +4499,7 @@
     <mergeCell ref="I26:I27"/>
     <mergeCell ref="I24:M24"/>
     <mergeCell ref="N24:O24"/>
+    <mergeCell ref="O21:O22"/>
     <mergeCell ref="C35:O35"/>
     <mergeCell ref="C36:O36"/>
     <mergeCell ref="D34:K34"/>
@@ -4473,8 +4520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{910156E5-166D-4067-94E6-30C47C096607}">
   <dimension ref="B1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18:M20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4493,181 +4540,181 @@
     <row r="1" spans="2:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="165" t="s">
+      <c r="C2" s="166" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
-      <c r="J2" s="165"/>
-      <c r="K2" s="165"/>
-      <c r="L2" s="165"/>
-      <c r="M2" s="165"/>
-      <c r="N2" s="165"/>
-      <c r="O2" s="165"/>
-      <c r="P2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="166"/>
+      <c r="H2" s="166"/>
+      <c r="I2" s="166"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="166"/>
+      <c r="M2" s="166"/>
+      <c r="N2" s="166"/>
+      <c r="O2" s="166"/>
+      <c r="P2" s="167"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
-      <c r="C3" s="168"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168"/>
-      <c r="H3" s="168"/>
-      <c r="I3" s="168"/>
-      <c r="J3" s="168"/>
-      <c r="K3" s="168"/>
-      <c r="L3" s="168"/>
-      <c r="M3" s="168"/>
-      <c r="N3" s="168"/>
-      <c r="O3" s="168"/>
-      <c r="P3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
+      <c r="E3" s="169"/>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="169"/>
+      <c r="L3" s="169"/>
+      <c r="M3" s="169"/>
+      <c r="N3" s="169"/>
+      <c r="O3" s="169"/>
+      <c r="P3" s="170"/>
     </row>
     <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
-      <c r="C4" s="171"/>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
-      <c r="F4" s="171"/>
-      <c r="G4" s="171"/>
-      <c r="H4" s="171"/>
-      <c r="I4" s="171"/>
-      <c r="J4" s="171"/>
-      <c r="K4" s="171"/>
-      <c r="L4" s="171"/>
-      <c r="M4" s="171"/>
-      <c r="N4" s="171"/>
-      <c r="O4" s="171"/>
-      <c r="P4" s="172"/>
+      <c r="C4" s="172"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="172"/>
+      <c r="F4" s="172"/>
+      <c r="G4" s="172"/>
+      <c r="H4" s="172"/>
+      <c r="I4" s="172"/>
+      <c r="J4" s="172"/>
+      <c r="K4" s="172"/>
+      <c r="L4" s="172"/>
+      <c r="M4" s="172"/>
+      <c r="N4" s="172"/>
+      <c r="O4" s="172"/>
+      <c r="P4" s="173"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="206" t="s">
+      <c r="C5" s="208" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="207"/>
-      <c r="E5" s="207"/>
-      <c r="F5" s="207"/>
-      <c r="G5" s="207"/>
-      <c r="H5" s="207"/>
-      <c r="I5" s="207"/>
-      <c r="J5" s="207"/>
-      <c r="K5" s="207"/>
-      <c r="L5" s="207"/>
-      <c r="M5" s="207"/>
-      <c r="N5" s="207"/>
-      <c r="O5" s="207"/>
-      <c r="P5" s="208"/>
+      <c r="D5" s="209"/>
+      <c r="E5" s="209"/>
+      <c r="F5" s="209"/>
+      <c r="G5" s="209"/>
+      <c r="H5" s="209"/>
+      <c r="I5" s="209"/>
+      <c r="J5" s="209"/>
+      <c r="K5" s="209"/>
+      <c r="L5" s="209"/>
+      <c r="M5" s="209"/>
+      <c r="N5" s="209"/>
+      <c r="O5" s="209"/>
+      <c r="P5" s="210"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
-      <c r="C6" s="209"/>
-      <c r="D6" s="209"/>
-      <c r="E6" s="209"/>
-      <c r="F6" s="209"/>
-      <c r="G6" s="209"/>
-      <c r="H6" s="209"/>
-      <c r="I6" s="209"/>
-      <c r="J6" s="209"/>
-      <c r="K6" s="209"/>
-      <c r="L6" s="209"/>
-      <c r="M6" s="209"/>
-      <c r="N6" s="209"/>
-      <c r="O6" s="209"/>
-      <c r="P6" s="210"/>
+      <c r="C6" s="211"/>
+      <c r="D6" s="211"/>
+      <c r="E6" s="211"/>
+      <c r="F6" s="211"/>
+      <c r="G6" s="211"/>
+      <c r="H6" s="211"/>
+      <c r="I6" s="211"/>
+      <c r="J6" s="211"/>
+      <c r="K6" s="211"/>
+      <c r="L6" s="211"/>
+      <c r="M6" s="211"/>
+      <c r="N6" s="211"/>
+      <c r="O6" s="211"/>
+      <c r="P6" s="212"/>
     </row>
     <row r="7" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
-      <c r="C7" s="211"/>
-      <c r="D7" s="211"/>
-      <c r="E7" s="211"/>
-      <c r="F7" s="211"/>
-      <c r="G7" s="211"/>
-      <c r="H7" s="211"/>
-      <c r="I7" s="211"/>
-      <c r="J7" s="211"/>
-      <c r="K7" s="211"/>
-      <c r="L7" s="211"/>
-      <c r="M7" s="211"/>
-      <c r="N7" s="211"/>
-      <c r="O7" s="211"/>
-      <c r="P7" s="212"/>
+      <c r="C7" s="213"/>
+      <c r="D7" s="213"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="213"/>
+      <c r="G7" s="213"/>
+      <c r="H7" s="213"/>
+      <c r="I7" s="213"/>
+      <c r="J7" s="213"/>
+      <c r="K7" s="213"/>
+      <c r="L7" s="213"/>
+      <c r="M7" s="213"/>
+      <c r="N7" s="213"/>
+      <c r="O7" s="213"/>
+      <c r="P7" s="214"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-      <c r="C8" s="163" t="s">
+      <c r="C8" s="164" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="163"/>
-      <c r="H8" s="163"/>
-      <c r="I8" s="163"/>
-      <c r="J8" s="163"/>
-      <c r="K8" s="163"/>
-      <c r="L8" s="163"/>
-      <c r="M8" s="163"/>
-      <c r="N8" s="163"/>
-      <c r="O8" s="163"/>
-      <c r="P8" s="173"/>
+      <c r="D8" s="164"/>
+      <c r="E8" s="164"/>
+      <c r="F8" s="164"/>
+      <c r="G8" s="164"/>
+      <c r="H8" s="164"/>
+      <c r="I8" s="164"/>
+      <c r="J8" s="164"/>
+      <c r="K8" s="164"/>
+      <c r="L8" s="164"/>
+      <c r="M8" s="164"/>
+      <c r="N8" s="164"/>
+      <c r="O8" s="164"/>
+      <c r="P8" s="174"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
-      <c r="C9" s="204" t="s">
+      <c r="C9" s="206" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="200"/>
-      <c r="E9" s="200"/>
-      <c r="F9" s="200"/>
-      <c r="G9" s="200"/>
-      <c r="H9" s="200"/>
-      <c r="I9" s="200"/>
-      <c r="J9" s="200"/>
-      <c r="K9" s="200"/>
-      <c r="L9" s="200"/>
-      <c r="M9" s="200"/>
-      <c r="N9" s="200"/>
-      <c r="O9" s="200"/>
-      <c r="P9" s="201"/>
+      <c r="D9" s="202"/>
+      <c r="E9" s="202"/>
+      <c r="F9" s="202"/>
+      <c r="G9" s="202"/>
+      <c r="H9" s="202"/>
+      <c r="I9" s="202"/>
+      <c r="J9" s="202"/>
+      <c r="K9" s="202"/>
+      <c r="L9" s="202"/>
+      <c r="M9" s="202"/>
+      <c r="N9" s="202"/>
+      <c r="O9" s="202"/>
+      <c r="P9" s="203"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
-      <c r="C10" s="204"/>
-      <c r="D10" s="200"/>
-      <c r="E10" s="200"/>
-      <c r="F10" s="200"/>
-      <c r="G10" s="200"/>
-      <c r="H10" s="200"/>
-      <c r="I10" s="200"/>
-      <c r="J10" s="200"/>
-      <c r="K10" s="200"/>
-      <c r="L10" s="200"/>
-      <c r="M10" s="200"/>
-      <c r="N10" s="200"/>
-      <c r="O10" s="200"/>
-      <c r="P10" s="201"/>
+      <c r="C10" s="206"/>
+      <c r="D10" s="202"/>
+      <c r="E10" s="202"/>
+      <c r="F10" s="202"/>
+      <c r="G10" s="202"/>
+      <c r="H10" s="202"/>
+      <c r="I10" s="202"/>
+      <c r="J10" s="202"/>
+      <c r="K10" s="202"/>
+      <c r="L10" s="202"/>
+      <c r="M10" s="202"/>
+      <c r="N10" s="202"/>
+      <c r="O10" s="202"/>
+      <c r="P10" s="203"/>
     </row>
     <row r="11" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
-      <c r="C11" s="205"/>
-      <c r="D11" s="202"/>
-      <c r="E11" s="202"/>
-      <c r="F11" s="202"/>
-      <c r="G11" s="202"/>
-      <c r="H11" s="202"/>
-      <c r="I11" s="202"/>
-      <c r="J11" s="202"/>
-      <c r="K11" s="202"/>
-      <c r="L11" s="202"/>
-      <c r="M11" s="202"/>
-      <c r="N11" s="202"/>
-      <c r="O11" s="202"/>
-      <c r="P11" s="203"/>
+      <c r="C11" s="207"/>
+      <c r="D11" s="204"/>
+      <c r="E11" s="204"/>
+      <c r="F11" s="204"/>
+      <c r="G11" s="204"/>
+      <c r="H11" s="204"/>
+      <c r="I11" s="204"/>
+      <c r="J11" s="204"/>
+      <c r="K11" s="204"/>
+      <c r="L11" s="204"/>
+      <c r="M11" s="204"/>
+      <c r="N11" s="204"/>
+      <c r="O11" s="204"/>
+      <c r="P11" s="205"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
@@ -4690,56 +4737,56 @@
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
-      <c r="C13" s="200" t="s">
+      <c r="C13" s="202" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="200"/>
-      <c r="E13" s="200"/>
-      <c r="F13" s="200"/>
-      <c r="G13" s="200"/>
-      <c r="H13" s="200"/>
-      <c r="I13" s="200"/>
-      <c r="J13" s="200"/>
-      <c r="K13" s="200"/>
-      <c r="L13" s="200"/>
-      <c r="M13" s="200"/>
-      <c r="N13" s="200"/>
-      <c r="O13" s="200"/>
-      <c r="P13" s="201"/>
+      <c r="D13" s="202"/>
+      <c r="E13" s="202"/>
+      <c r="F13" s="202"/>
+      <c r="G13" s="202"/>
+      <c r="H13" s="202"/>
+      <c r="I13" s="202"/>
+      <c r="J13" s="202"/>
+      <c r="K13" s="202"/>
+      <c r="L13" s="202"/>
+      <c r="M13" s="202"/>
+      <c r="N13" s="202"/>
+      <c r="O13" s="202"/>
+      <c r="P13" s="203"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
-      <c r="C14" s="200"/>
-      <c r="D14" s="200"/>
-      <c r="E14" s="200"/>
-      <c r="F14" s="200"/>
-      <c r="G14" s="200"/>
-      <c r="H14" s="200"/>
-      <c r="I14" s="200"/>
-      <c r="J14" s="200"/>
-      <c r="K14" s="200"/>
-      <c r="L14" s="200"/>
-      <c r="M14" s="200"/>
-      <c r="N14" s="200"/>
-      <c r="O14" s="200"/>
-      <c r="P14" s="201"/>
+      <c r="C14" s="202"/>
+      <c r="D14" s="202"/>
+      <c r="E14" s="202"/>
+      <c r="F14" s="202"/>
+      <c r="G14" s="202"/>
+      <c r="H14" s="202"/>
+      <c r="I14" s="202"/>
+      <c r="J14" s="202"/>
+      <c r="K14" s="202"/>
+      <c r="L14" s="202"/>
+      <c r="M14" s="202"/>
+      <c r="N14" s="202"/>
+      <c r="O14" s="202"/>
+      <c r="P14" s="203"/>
     </row>
     <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
-      <c r="C15" s="202"/>
-      <c r="D15" s="202"/>
-      <c r="E15" s="202"/>
-      <c r="F15" s="202"/>
-      <c r="G15" s="202"/>
-      <c r="H15" s="202"/>
-      <c r="I15" s="202"/>
-      <c r="J15" s="202"/>
-      <c r="K15" s="202"/>
-      <c r="L15" s="202"/>
-      <c r="M15" s="202"/>
-      <c r="N15" s="202"/>
-      <c r="O15" s="202"/>
-      <c r="P15" s="203"/>
+      <c r="C15" s="204"/>
+      <c r="D15" s="204"/>
+      <c r="E15" s="204"/>
+      <c r="F15" s="204"/>
+      <c r="G15" s="204"/>
+      <c r="H15" s="204"/>
+      <c r="I15" s="204"/>
+      <c r="J15" s="204"/>
+      <c r="K15" s="204"/>
+      <c r="L15" s="204"/>
+      <c r="M15" s="204"/>
+      <c r="N15" s="204"/>
+      <c r="O15" s="204"/>
+      <c r="P15" s="205"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
@@ -4776,13 +4823,13 @@
       <c r="D18" s="120"/>
       <c r="E18" s="120"/>
       <c r="F18" s="120"/>
-      <c r="G18" s="183"/>
-      <c r="H18" s="197"/>
+      <c r="G18" s="186"/>
+      <c r="H18" s="199"/>
       <c r="I18" s="120"/>
       <c r="J18" s="120"/>
       <c r="K18" s="120"/>
       <c r="L18" s="120"/>
-      <c r="M18" s="183"/>
+      <c r="M18" s="186"/>
       <c r="N18" s="4"/>
       <c r="P18" s="5"/>
     </row>
@@ -4792,13 +4839,13 @@
       <c r="D19" s="120"/>
       <c r="E19" s="120"/>
       <c r="F19" s="120"/>
-      <c r="G19" s="183"/>
-      <c r="H19" s="197"/>
+      <c r="G19" s="186"/>
+      <c r="H19" s="199"/>
       <c r="I19" s="120"/>
       <c r="J19" s="120"/>
       <c r="K19" s="120"/>
       <c r="L19" s="120"/>
-      <c r="M19" s="183"/>
+      <c r="M19" s="186"/>
       <c r="N19" s="4"/>
       <c r="P19" s="5"/>
     </row>
@@ -4817,7 +4864,7 @@
       <c r="M20" s="102"/>
       <c r="N20" s="103"/>
       <c r="O20" s="104"/>
-      <c r="P20" s="192"/>
+      <c r="P20" s="194"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
@@ -4838,14 +4885,14 @@
       <c r="M21" s="76"/>
       <c r="N21" s="103"/>
       <c r="O21" s="104"/>
-      <c r="P21" s="192"/>
+      <c r="P21" s="194"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="G22" s="5"/>
       <c r="N22" s="103"/>
       <c r="O22" s="104"/>
-      <c r="P22" s="192"/>
+      <c r="P22" s="194"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
@@ -4855,18 +4902,18 @@
       <c r="D23" s="120"/>
       <c r="E23" s="120"/>
       <c r="F23" s="120"/>
-      <c r="G23" s="183"/>
-      <c r="H23" s="197">
+      <c r="G23" s="186"/>
+      <c r="H23" s="199">
         <v>10398004506</v>
       </c>
       <c r="I23" s="120"/>
       <c r="J23" s="120"/>
       <c r="K23" s="120"/>
       <c r="L23" s="120"/>
-      <c r="M23" s="183"/>
+      <c r="M23" s="186"/>
       <c r="N23" s="103"/>
       <c r="O23" s="104"/>
-      <c r="P23" s="192"/>
+      <c r="P23" s="194"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
@@ -4874,16 +4921,16 @@
       <c r="D24" s="120"/>
       <c r="E24" s="120"/>
       <c r="F24" s="120"/>
-      <c r="G24" s="183"/>
-      <c r="H24" s="197"/>
+      <c r="G24" s="186"/>
+      <c r="H24" s="199"/>
       <c r="I24" s="120"/>
       <c r="J24" s="120"/>
       <c r="K24" s="120"/>
       <c r="L24" s="120"/>
-      <c r="M24" s="183"/>
+      <c r="M24" s="186"/>
       <c r="N24" s="103"/>
       <c r="O24" s="104"/>
-      <c r="P24" s="192"/>
+      <c r="P24" s="194"/>
     </row>
     <row r="25" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6"/>
@@ -4929,26 +4976,30 @@
       <c r="B27" s="4"/>
       <c r="G27" s="5"/>
       <c r="M27" s="5"/>
-      <c r="N27" s="197"/>
+      <c r="N27" s="199">
+        <v>1750102610</v>
+      </c>
       <c r="O27" s="120"/>
-      <c r="P27" s="183"/>
+      <c r="P27" s="186"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="120"/>
+      <c r="C28" s="120" t="s">
+        <v>87</v>
+      </c>
       <c r="D28" s="120"/>
       <c r="E28" s="120"/>
       <c r="F28" s="120"/>
-      <c r="G28" s="183"/>
-      <c r="H28" s="197"/>
+      <c r="G28" s="186"/>
+      <c r="H28" s="199"/>
       <c r="I28" s="120"/>
       <c r="J28" s="120"/>
       <c r="K28" s="120"/>
       <c r="L28" s="120"/>
-      <c r="M28" s="183"/>
-      <c r="N28" s="197"/>
+      <c r="M28" s="186"/>
+      <c r="N28" s="199"/>
       <c r="O28" s="120"/>
-      <c r="P28" s="183"/>
+      <c r="P28" s="186"/>
     </row>
     <row r="29" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6"/>
@@ -4994,44 +5045,44 @@
       <c r="B31" s="4"/>
       <c r="G31" s="5"/>
       <c r="M31" s="5"/>
-      <c r="N31" s="197" t="s">
+      <c r="N31" s="199" t="s">
         <v>80</v>
       </c>
       <c r="O31" s="120"/>
-      <c r="P31" s="183"/>
+      <c r="P31" s="186"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
-      <c r="C32" s="198"/>
-      <c r="D32" s="198"/>
+      <c r="C32" s="200"/>
+      <c r="D32" s="200"/>
       <c r="E32" s="120" t="s">
         <v>51</v>
       </c>
       <c r="F32" s="120"/>
-      <c r="G32" s="183"/>
-      <c r="H32" s="197"/>
-      <c r="I32" s="120"/>
-      <c r="J32" s="120"/>
-      <c r="K32" s="120"/>
-      <c r="L32" s="120"/>
-      <c r="M32" s="183"/>
-      <c r="N32" s="197"/>
+      <c r="G32" s="186"/>
+      <c r="H32" s="218"/>
+      <c r="I32" s="219"/>
+      <c r="J32" s="219"/>
+      <c r="K32" s="219"/>
+      <c r="L32" s="219"/>
+      <c r="M32" s="220"/>
+      <c r="N32" s="199"/>
       <c r="O32" s="120"/>
-      <c r="P32" s="183"/>
+      <c r="P32" s="186"/>
     </row>
     <row r="33" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
-      <c r="C33" s="199"/>
-      <c r="D33" s="199"/>
+      <c r="C33" s="201"/>
+      <c r="D33" s="201"/>
       <c r="E33" s="101"/>
       <c r="F33" s="101"/>
       <c r="G33" s="102"/>
-      <c r="H33" s="132"/>
-      <c r="I33" s="101"/>
-      <c r="J33" s="101"/>
-      <c r="K33" s="101"/>
-      <c r="L33" s="101"/>
-      <c r="M33" s="102"/>
+      <c r="H33" s="221"/>
+      <c r="I33" s="222"/>
+      <c r="J33" s="222"/>
+      <c r="K33" s="222"/>
+      <c r="L33" s="222"/>
+      <c r="M33" s="223"/>
       <c r="N33" s="132"/>
       <c r="O33" s="101"/>
       <c r="P33" s="102"/>
@@ -5061,30 +5112,30 @@
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
-      <c r="C35" s="193"/>
-      <c r="D35" s="193"/>
-      <c r="E35" s="193"/>
-      <c r="F35" s="193"/>
-      <c r="G35" s="194"/>
+      <c r="C35" s="195"/>
+      <c r="D35" s="195"/>
+      <c r="E35" s="195"/>
+      <c r="F35" s="195"/>
+      <c r="G35" s="196"/>
       <c r="H35" s="103"/>
       <c r="I35" s="104"/>
       <c r="J35" s="104"/>
       <c r="K35" s="104"/>
       <c r="L35" s="104"/>
-      <c r="M35" s="192"/>
-      <c r="N35" s="197" t="s">
+      <c r="M35" s="194"/>
+      <c r="N35" s="199" t="s">
         <v>65</v>
       </c>
       <c r="O35" s="120"/>
-      <c r="P35" s="183"/>
+      <c r="P35" s="186"/>
     </row>
     <row r="36" spans="2:16" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="6"/>
-      <c r="C36" s="195"/>
-      <c r="D36" s="195"/>
-      <c r="E36" s="195"/>
-      <c r="F36" s="195"/>
-      <c r="G36" s="196"/>
+      <c r="C36" s="197"/>
+      <c r="D36" s="197"/>
+      <c r="E36" s="197"/>
+      <c r="F36" s="197"/>
+      <c r="G36" s="198"/>
       <c r="H36" s="105"/>
       <c r="I36" s="106"/>
       <c r="J36" s="106"/>

</xml_diff>